<commit_message>
Final styling to excel sheets
</commit_message>
<xml_diff>
--- a/a2_q3.xlsx
+++ b/a2_q3.xlsx
@@ -25,7 +25,7 @@
     <t xml:space="preserve">Assignment 2: Question 3 Data – SIDDHARTH GUPTA – 301327469</t>
   </si>
   <si>
-    <t xml:space="preserve">ITERATION #1</t>
+    <t xml:space="preserve">ITERATION #1 – SOLUTIONS OF EACH PROBLEM ARE INDICATED IN THE RED CELLS !</t>
   </si>
   <si>
     <t xml:space="preserve">Friendship graph #</t>
@@ -64,16 +64,16 @@
     <t xml:space="preserve">Median =</t>
   </si>
   <si>
-    <t xml:space="preserve">ITERATION #2</t>
+    <t xml:space="preserve">ITERATION #2 – SOLUTIONS OF EACH PROBLEM ARE INDICATED IN THE RED CELLS !</t>
   </si>
   <si>
-    <t xml:space="preserve">ITERATION #3</t>
+    <t xml:space="preserve">ITERATION #3 – SOLUTIONS OF EACH PROBLEM ARE INDICATED IN THE RED CELLS !</t>
   </si>
   <si>
-    <t xml:space="preserve">ITERATION #4</t>
+    <t xml:space="preserve">ITERATION #4 – SOLUTIONS OF EACH PROBLEM ARE INDICATED IN THE RED CELLS !</t>
   </si>
   <si>
-    <t xml:space="preserve">ITERATION #5</t>
+    <t xml:space="preserve">ITERATION #5 – SOLUTIONS OF EACH PROBLEM ARE INDICATED IN THE RED CELLS !</t>
   </si>
 </sst>
 </file>
@@ -83,7 +83,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="8">
+  <fonts count="7">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -123,13 +123,6 @@
       <charset val="1"/>
     </font>
     <font>
-      <b val="true"/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-    </font>
-    <font>
       <sz val="11"/>
       <color rgb="FFFFFFFF"/>
       <name val="Calibri"/>
@@ -137,7 +130,7 @@
       <charset val="1"/>
     </font>
   </fonts>
-  <fills count="9">
+  <fills count="10">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -160,6 +153,12 @@
       <patternFill patternType="solid">
         <fgColor rgb="FF62A73B"/>
         <bgColor rgb="FF808000"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFED1C24"/>
+        <bgColor rgb="FF993300"/>
       </patternFill>
     </fill>
     <fill>
@@ -187,7 +186,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border diagonalUp="false" diagonalDown="false">
       <left/>
       <right/>
@@ -208,6 +207,13 @@
       <bottom style="hair">
         <color rgb="FFFFFFFF"/>
       </bottom>
+      <diagonal/>
+    </border>
+    <border diagonalUp="false" diagonalDown="false">
+      <left style="hair"/>
+      <right style="hair"/>
+      <top style="hair"/>
+      <bottom style="hair"/>
       <diagonal/>
     </border>
   </borders>
@@ -241,11 +247,11 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -253,7 +259,7 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="5" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="5" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -261,19 +267,19 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="7" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="7" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="8" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="8" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="5" fillId="9" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="8" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -290,7 +296,7 @@
     <indexedColors>
       <rgbColor rgb="FF000000"/>
       <rgbColor rgb="FFFFFFFF"/>
-      <rgbColor rgb="FFFF0000"/>
+      <rgbColor rgb="FFED1C24"/>
       <rgbColor rgb="FF00FF00"/>
       <rgbColor rgb="FF0000FF"/>
       <rgbColor rgb="FFFFFF00"/>
@@ -356,8 +362,8 @@
   </sheetPr>
   <dimension ref="A1:H61"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A3" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="60" zoomScaleNormal="60" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="E23" activeCellId="0" sqref="E23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -366,7 +372,7 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="27.45"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="26.51"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="47.11"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="29.16"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="29.17"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="30.87"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="37.47"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="24.94"/>
@@ -426,7 +432,7 @@
       <c r="F4" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="G4" s="3" t="s">
+      <c r="G4" s="4" t="s">
         <v>8</v>
       </c>
       <c r="H4" s="3" t="s">
@@ -434,146 +440,146 @@
       </c>
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="4" t="n">
+      <c r="A5" s="5" t="n">
         <v>1</v>
       </c>
-      <c r="B5" s="5" t="n">
-        <v>30</v>
-      </c>
-      <c r="C5" s="4" t="n">
+      <c r="B5" s="6" t="n">
+        <v>30</v>
+      </c>
+      <c r="C5" s="5" t="n">
         <v>0.1</v>
       </c>
-      <c r="D5" s="5" t="n">
+      <c r="D5" s="6" t="n">
         <v>0.00172305107116699</v>
       </c>
-      <c r="E5" s="4" t="n">
+      <c r="E5" s="5" t="n">
         <v>46</v>
       </c>
-      <c r="F5" s="5" t="n">
+      <c r="F5" s="6" t="n">
         <v>14</v>
       </c>
       <c r="G5" s="4" t="n">
         <v>3</v>
       </c>
-      <c r="H5" s="5" t="n">
+      <c r="H5" s="6" t="n">
         <v>96</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="4" t="n">
+      <c r="A6" s="5" t="n">
         <v>2</v>
       </c>
-      <c r="B6" s="5" t="n">
-        <v>30</v>
-      </c>
-      <c r="C6" s="4" t="n">
+      <c r="B6" s="6" t="n">
+        <v>30</v>
+      </c>
+      <c r="C6" s="5" t="n">
         <v>0.2</v>
       </c>
-      <c r="D6" s="5" t="n">
+      <c r="D6" s="6" t="n">
         <v>0.00849270820617676</v>
       </c>
-      <c r="E6" s="4" t="n">
+      <c r="E6" s="5" t="n">
         <v>270</v>
       </c>
-      <c r="F6" s="5" t="n">
+      <c r="F6" s="6" t="n">
         <v>213</v>
       </c>
       <c r="G6" s="4" t="n">
         <v>4</v>
       </c>
-      <c r="H6" s="5" t="n">
+      <c r="H6" s="6" t="n">
         <v>802</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="4" t="n">
-        <v>3</v>
-      </c>
-      <c r="B7" s="5" t="n">
-        <v>30</v>
-      </c>
-      <c r="C7" s="4" t="n">
+      <c r="A7" s="5" t="n">
+        <v>3</v>
+      </c>
+      <c r="B7" s="6" t="n">
+        <v>30</v>
+      </c>
+      <c r="C7" s="5" t="n">
         <v>0.3</v>
       </c>
-      <c r="D7" s="5" t="n">
+      <c r="D7" s="6" t="n">
         <v>0.0283396244049072</v>
       </c>
-      <c r="E7" s="4" t="n">
+      <c r="E7" s="5" t="n">
         <v>758</v>
       </c>
-      <c r="F7" s="5" t="n">
+      <c r="F7" s="6" t="n">
         <v>618</v>
       </c>
       <c r="G7" s="4" t="n">
         <v>5</v>
       </c>
-      <c r="H7" s="5" t="n">
+      <c r="H7" s="6" t="n">
         <v>3585</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="4" t="n">
+      <c r="A8" s="5" t="n">
         <v>4</v>
       </c>
-      <c r="B8" s="5" t="n">
-        <v>30</v>
-      </c>
-      <c r="C8" s="4" t="n">
+      <c r="B8" s="6" t="n">
+        <v>30</v>
+      </c>
+      <c r="C8" s="5" t="n">
         <v>0.4</v>
       </c>
-      <c r="D8" s="5" t="n">
+      <c r="D8" s="6" t="n">
         <v>1.08942937850952</v>
       </c>
-      <c r="E8" s="4" t="n">
+      <c r="E8" s="5" t="n">
         <v>31743</v>
       </c>
-      <c r="F8" s="5" t="n">
+      <c r="F8" s="6" t="n">
         <v>26778</v>
       </c>
       <c r="G8" s="4" t="n">
         <v>6</v>
       </c>
-      <c r="H8" s="5" t="n">
+      <c r="H8" s="6" t="n">
         <v>135460</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="4" t="n">
-        <v>5</v>
-      </c>
-      <c r="B9" s="5" t="n">
-        <v>30</v>
-      </c>
-      <c r="C9" s="4" t="n">
+      <c r="A9" s="5" t="n">
+        <v>5</v>
+      </c>
+      <c r="B9" s="6" t="n">
+        <v>30</v>
+      </c>
+      <c r="C9" s="5" t="n">
         <v>0.5</v>
       </c>
-      <c r="D9" s="5" t="n">
+      <c r="D9" s="6" t="n">
         <v>10.465784072876</v>
       </c>
-      <c r="E9" s="4" t="n">
+      <c r="E9" s="5" t="n">
         <v>278318</v>
       </c>
-      <c r="F9" s="5" t="n">
+      <c r="F9" s="6" t="n">
         <v>237620</v>
       </c>
       <c r="G9" s="4" t="n">
         <v>7</v>
       </c>
-      <c r="H9" s="5" t="n">
+      <c r="H9" s="6" t="n">
         <v>1184011</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="6" t="s">
+      <c r="A10" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="B10" s="6"/>
-      <c r="C10" s="6"/>
-      <c r="D10" s="7" t="n">
+      <c r="B10" s="7"/>
+      <c r="C10" s="7"/>
+      <c r="D10" s="8" t="n">
         <f aca="false">MIN(D5:D9)</f>
         <v>0.00172305107116699</v>
       </c>
-      <c r="E10" s="7" t="n">
+      <c r="E10" s="8" t="n">
         <f aca="false">MIN(E5:E9)</f>
         <v>46</v>
       </c>
@@ -585,88 +591,88 @@
         <f aca="false">MIN(G5:G9)</f>
         <v>3</v>
       </c>
-      <c r="H10" s="7" t="n">
+      <c r="H10" s="8" t="n">
         <f aca="false">MIN(H5:H9)</f>
         <v>96</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="6" t="s">
+      <c r="A11" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="B11" s="6"/>
-      <c r="C11" s="6"/>
-      <c r="D11" s="7" t="n">
+      <c r="B11" s="7"/>
+      <c r="C11" s="7"/>
+      <c r="D11" s="8" t="n">
         <f aca="false">MAX(D5:D9)</f>
         <v>10.465784072876</v>
       </c>
-      <c r="E11" s="7" t="n">
+      <c r="E11" s="8" t="n">
         <f aca="false">MAX(E5:E9)</f>
         <v>278318</v>
       </c>
-      <c r="F11" s="7" t="n">
+      <c r="F11" s="8" t="n">
         <f aca="false">MAX(F5:F9)</f>
         <v>237620</v>
       </c>
-      <c r="G11" s="7" t="n">
+      <c r="G11" s="8" t="n">
         <f aca="false">MAX(G5:G9)</f>
         <v>7</v>
       </c>
-      <c r="H11" s="7" t="n">
+      <c r="H11" s="8" t="n">
         <f aca="false">MAX(H5:H9)</f>
         <v>1184011</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="6" t="s">
+      <c r="A12" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="B12" s="6"/>
-      <c r="C12" s="6"/>
-      <c r="D12" s="7" t="n">
+      <c r="B12" s="7"/>
+      <c r="C12" s="7"/>
+      <c r="D12" s="8" t="n">
         <f aca="false">AVERAGE(D5:D9)</f>
         <v>2.31875376701355</v>
       </c>
-      <c r="E12" s="7" t="n">
+      <c r="E12" s="8" t="n">
         <f aca="false">AVERAGE(E5:E9)</f>
         <v>62227</v>
       </c>
-      <c r="F12" s="7" t="n">
+      <c r="F12" s="8" t="n">
         <f aca="false">AVERAGE(F5:F9)</f>
         <v>53048.6</v>
       </c>
-      <c r="G12" s="7" t="n">
+      <c r="G12" s="8" t="n">
         <f aca="false">AVERAGE(G5:G9)</f>
         <v>5</v>
       </c>
-      <c r="H12" s="7" t="n">
+      <c r="H12" s="8" t="n">
         <f aca="false">AVERAGE(H5:H9)</f>
         <v>264790.8</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="6" t="s">
+      <c r="A13" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="B13" s="6"/>
-      <c r="C13" s="6"/>
-      <c r="D13" s="7" t="n">
+      <c r="B13" s="7"/>
+      <c r="C13" s="7"/>
+      <c r="D13" s="8" t="n">
         <f aca="false">MEDIAN(D5:D9)</f>
         <v>0.0283396244049072</v>
       </c>
-      <c r="E13" s="7" t="n">
+      <c r="E13" s="8" t="n">
         <f aca="false">MEDIAN(E5:E9)</f>
         <v>758</v>
       </c>
-      <c r="F13" s="7" t="n">
+      <c r="F13" s="8" t="n">
         <f aca="false">MEDIAN(F5:F9)</f>
         <v>618</v>
       </c>
-      <c r="G13" s="7" t="n">
+      <c r="G13" s="8" t="n">
         <f aca="false">MEDIAN(G5:G9)</f>
         <v>5</v>
       </c>
-      <c r="H13" s="7" t="n">
+      <c r="H13" s="8" t="n">
         <f aca="false">MEDIAN(H5:H9)</f>
         <v>3585</v>
       </c>
@@ -702,7 +708,7 @@
       <c r="F16" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="G16" s="3" t="s">
+      <c r="G16" s="4" t="s">
         <v>8</v>
       </c>
       <c r="H16" s="3" t="s">
@@ -710,239 +716,239 @@
       </c>
     </row>
     <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="4" t="n">
+      <c r="A17" s="5" t="n">
         <v>1</v>
       </c>
-      <c r="B17" s="5" t="n">
-        <v>30</v>
-      </c>
-      <c r="C17" s="4" t="n">
+      <c r="B17" s="6" t="n">
+        <v>30</v>
+      </c>
+      <c r="C17" s="5" t="n">
         <v>0.1</v>
       </c>
-      <c r="D17" s="5" t="n">
+      <c r="D17" s="6" t="n">
         <v>0.00152468681335449</v>
       </c>
-      <c r="E17" s="4" t="n">
+      <c r="E17" s="5" t="n">
         <v>42</v>
       </c>
-      <c r="F17" s="5" t="n">
+      <c r="F17" s="6" t="n">
         <v>11</v>
       </c>
       <c r="G17" s="4" t="n">
         <v>3</v>
       </c>
-      <c r="H17" s="5" t="n">
+      <c r="H17" s="6" t="n">
         <v>69</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="4" t="n">
+      <c r="A18" s="5" t="n">
         <v>2</v>
       </c>
-      <c r="B18" s="5" t="n">
-        <v>30</v>
-      </c>
-      <c r="C18" s="4" t="n">
+      <c r="B18" s="6" t="n">
+        <v>30</v>
+      </c>
+      <c r="C18" s="5" t="n">
         <v>0.2</v>
       </c>
-      <c r="D18" s="5" t="n">
+      <c r="D18" s="6" t="n">
         <v>0.00496077537536621</v>
       </c>
-      <c r="E18" s="4" t="n">
+      <c r="E18" s="5" t="n">
         <v>136</v>
       </c>
-      <c r="F18" s="5" t="n">
+      <c r="F18" s="6" t="n">
         <v>93</v>
       </c>
       <c r="G18" s="4" t="n">
         <v>4</v>
       </c>
-      <c r="H18" s="5" t="n">
+      <c r="H18" s="6" t="n">
         <v>471</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="4" t="n">
-        <v>3</v>
-      </c>
-      <c r="B19" s="5" t="n">
-        <v>30</v>
-      </c>
-      <c r="C19" s="4" t="n">
+      <c r="A19" s="5" t="n">
+        <v>3</v>
+      </c>
+      <c r="B19" s="6" t="n">
+        <v>30</v>
+      </c>
+      <c r="C19" s="5" t="n">
         <v>0.3</v>
       </c>
-      <c r="D19" s="5" t="n">
+      <c r="D19" s="6" t="n">
         <v>0.01119065284729</v>
       </c>
-      <c r="E19" s="4" t="n">
+      <c r="E19" s="5" t="n">
         <v>282</v>
       </c>
-      <c r="F19" s="5" t="n">
+      <c r="F19" s="6" t="n">
         <v>209</v>
       </c>
       <c r="G19" s="4" t="n">
         <v>5</v>
       </c>
-      <c r="H19" s="5" t="n">
+      <c r="H19" s="6" t="n">
         <v>1631</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="4" t="n">
+      <c r="A20" s="5" t="n">
         <v>4</v>
       </c>
-      <c r="B20" s="5" t="n">
-        <v>30</v>
-      </c>
-      <c r="C20" s="4" t="n">
+      <c r="B20" s="6" t="n">
+        <v>30</v>
+      </c>
+      <c r="C20" s="5" t="n">
         <v>0.4</v>
       </c>
-      <c r="D20" s="5" t="n">
+      <c r="D20" s="6" t="n">
         <v>0.489648342132568</v>
       </c>
-      <c r="E20" s="4" t="n">
+      <c r="E20" s="5" t="n">
         <v>15095</v>
       </c>
-      <c r="F20" s="5" t="n">
+      <c r="F20" s="6" t="n">
         <v>12950</v>
       </c>
       <c r="G20" s="4" t="n">
         <v>6</v>
       </c>
-      <c r="H20" s="5" t="n">
+      <c r="H20" s="6" t="n">
         <v>68882</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="4" t="n">
-        <v>5</v>
-      </c>
-      <c r="B21" s="5" t="n">
-        <v>30</v>
-      </c>
-      <c r="C21" s="4" t="n">
+      <c r="A21" s="5" t="n">
+        <v>5</v>
+      </c>
+      <c r="B21" s="6" t="n">
+        <v>30</v>
+      </c>
+      <c r="C21" s="5" t="n">
         <v>0.5</v>
       </c>
-      <c r="D21" s="5" t="n">
+      <c r="D21" s="6" t="n">
         <v>3.83439302444458</v>
       </c>
-      <c r="E21" s="4" t="n">
+      <c r="E21" s="5" t="n">
         <v>114241</v>
       </c>
-      <c r="F21" s="5" t="n">
+      <c r="F21" s="6" t="n">
         <v>97248</v>
       </c>
       <c r="G21" s="4" t="n">
         <v>7</v>
       </c>
-      <c r="H21" s="5" t="n">
+      <c r="H21" s="6" t="n">
         <v>508638</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A22" s="6" t="s">
+      <c r="A22" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="B22" s="6"/>
-      <c r="C22" s="6"/>
-      <c r="D22" s="7" t="n">
+      <c r="B22" s="7"/>
+      <c r="C22" s="7"/>
+      <c r="D22" s="8" t="n">
         <f aca="false">MIN(D17:D21)</f>
         <v>0.00152468681335449</v>
       </c>
-      <c r="E22" s="7" t="n">
+      <c r="E22" s="8" t="n">
         <f aca="false">MIN(E17:E21)</f>
         <v>42</v>
       </c>
-      <c r="F22" s="7" t="n">
+      <c r="F22" s="8" t="n">
         <f aca="false">MIN(F17:F21)</f>
         <v>11</v>
       </c>
-      <c r="G22" s="7" t="n">
+      <c r="G22" s="8" t="n">
         <f aca="false">MIN(G17:G21)</f>
         <v>3</v>
       </c>
-      <c r="H22" s="7" t="n">
+      <c r="H22" s="8" t="n">
         <f aca="false">MIN(H17:H21)</f>
         <v>69</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A23" s="6" t="s">
+      <c r="A23" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="B23" s="6"/>
-      <c r="C23" s="6"/>
-      <c r="D23" s="7" t="n">
+      <c r="B23" s="7"/>
+      <c r="C23" s="7"/>
+      <c r="D23" s="8" t="n">
         <f aca="false">MAX(D17:D21)</f>
         <v>3.83439302444458</v>
       </c>
-      <c r="E23" s="7" t="n">
+      <c r="E23" s="8" t="n">
         <f aca="false">MAX(E17:E21)</f>
         <v>114241</v>
       </c>
-      <c r="F23" s="7" t="n">
+      <c r="F23" s="8" t="n">
         <f aca="false">MAX(F17:F21)</f>
         <v>97248</v>
       </c>
-      <c r="G23" s="7" t="n">
+      <c r="G23" s="8" t="n">
         <f aca="false">MAX(G17:G21)</f>
         <v>7</v>
       </c>
-      <c r="H23" s="7" t="n">
+      <c r="H23" s="8" t="n">
         <f aca="false">MAX(H17:H21)</f>
         <v>508638</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A24" s="6" t="s">
+      <c r="A24" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="B24" s="6"/>
-      <c r="C24" s="6"/>
-      <c r="D24" s="7" t="n">
+      <c r="B24" s="7"/>
+      <c r="C24" s="7"/>
+      <c r="D24" s="8" t="n">
         <f aca="false">AVERAGE(D17:D21)</f>
         <v>0.868343496322632</v>
       </c>
-      <c r="E24" s="7" t="n">
+      <c r="E24" s="8" t="n">
         <f aca="false">AVERAGE(E17:E21)</f>
         <v>25959.2</v>
       </c>
-      <c r="F24" s="7" t="n">
+      <c r="F24" s="8" t="n">
         <f aca="false">AVERAGE(F17:F21)</f>
         <v>22102.2</v>
       </c>
-      <c r="G24" s="7" t="n">
+      <c r="G24" s="8" t="n">
         <f aca="false">AVERAGE(G17:G21)</f>
         <v>5</v>
       </c>
-      <c r="H24" s="7" t="n">
+      <c r="H24" s="8" t="n">
         <f aca="false">AVERAGE(H17:H21)</f>
         <v>115938.2</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A25" s="6" t="s">
+      <c r="A25" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="B25" s="6"/>
-      <c r="C25" s="6"/>
-      <c r="D25" s="7" t="n">
+      <c r="B25" s="7"/>
+      <c r="C25" s="7"/>
+      <c r="D25" s="8" t="n">
         <f aca="false">MEDIAN(D17:D21)</f>
         <v>0.01119065284729</v>
       </c>
-      <c r="E25" s="7" t="n">
+      <c r="E25" s="8" t="n">
         <f aca="false">MEDIAN(E17:E21)</f>
         <v>282</v>
       </c>
-      <c r="F25" s="7" t="n">
+      <c r="F25" s="8" t="n">
         <f aca="false">MEDIAN(F17:F21)</f>
         <v>209</v>
       </c>
-      <c r="G25" s="7" t="n">
+      <c r="G25" s="8" t="n">
         <f aca="false">MEDIAN(G17:G21)</f>
         <v>5</v>
       </c>
-      <c r="H25" s="7" t="n">
+      <c r="H25" s="8" t="n">
         <f aca="false">MEDIAN(H17:H21)</f>
         <v>1631</v>
       </c>
@@ -978,7 +984,7 @@
       <c r="F28" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="G28" s="3" t="s">
+      <c r="G28" s="4" t="s">
         <v>8</v>
       </c>
       <c r="H28" s="3" t="s">
@@ -986,239 +992,239 @@
       </c>
     </row>
     <row r="29" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A29" s="4" t="n">
+      <c r="A29" s="5" t="n">
         <v>1</v>
       </c>
-      <c r="B29" s="5" t="n">
-        <v>30</v>
-      </c>
-      <c r="C29" s="4" t="n">
+      <c r="B29" s="6" t="n">
+        <v>30</v>
+      </c>
+      <c r="C29" s="5" t="n">
         <v>0.1</v>
       </c>
-      <c r="D29" s="5" t="n">
+      <c r="D29" s="6" t="n">
         <v>0.00157856941223145</v>
       </c>
-      <c r="E29" s="4" t="n">
+      <c r="E29" s="5" t="n">
         <v>44</v>
       </c>
-      <c r="F29" s="5" t="n">
+      <c r="F29" s="6" t="n">
         <v>13</v>
       </c>
       <c r="G29" s="4" t="n">
         <v>3</v>
       </c>
-      <c r="H29" s="5" t="n">
+      <c r="H29" s="6" t="n">
         <v>71</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A30" s="4" t="n">
+      <c r="A30" s="5" t="n">
         <v>2</v>
       </c>
-      <c r="B30" s="5" t="n">
-        <v>30</v>
-      </c>
-      <c r="C30" s="4" t="n">
+      <c r="B30" s="6" t="n">
+        <v>30</v>
+      </c>
+      <c r="C30" s="5" t="n">
         <v>0.2</v>
       </c>
-      <c r="D30" s="5" t="n">
+      <c r="D30" s="6" t="n">
         <v>0.00321245193481445</v>
       </c>
-      <c r="E30" s="4" t="n">
+      <c r="E30" s="5" t="n">
         <v>78</v>
       </c>
-      <c r="F30" s="5" t="n">
+      <c r="F30" s="6" t="n">
         <v>42</v>
       </c>
       <c r="G30" s="4" t="n">
         <v>4</v>
       </c>
-      <c r="H30" s="5" t="n">
+      <c r="H30" s="6" t="n">
         <v>299</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A31" s="4" t="n">
-        <v>3</v>
-      </c>
-      <c r="B31" s="5" t="n">
-        <v>30</v>
-      </c>
-      <c r="C31" s="4" t="n">
+      <c r="A31" s="5" t="n">
+        <v>3</v>
+      </c>
+      <c r="B31" s="6" t="n">
+        <v>30</v>
+      </c>
+      <c r="C31" s="5" t="n">
         <v>0.3</v>
       </c>
-      <c r="D31" s="5" t="n">
+      <c r="D31" s="6" t="n">
         <v>0.0594370365142822</v>
       </c>
-      <c r="E31" s="4" t="n">
+      <c r="E31" s="5" t="n">
         <v>1849</v>
       </c>
-      <c r="F31" s="5" t="n">
+      <c r="F31" s="6" t="n">
         <v>1523</v>
       </c>
       <c r="G31" s="4" t="n">
         <v>5</v>
       </c>
-      <c r="H31" s="5" t="n">
+      <c r="H31" s="6" t="n">
         <v>8251</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A32" s="4" t="n">
+      <c r="A32" s="5" t="n">
         <v>4</v>
       </c>
-      <c r="B32" s="5" t="n">
-        <v>30</v>
-      </c>
-      <c r="C32" s="4" t="n">
+      <c r="B32" s="6" t="n">
+        <v>30</v>
+      </c>
+      <c r="C32" s="5" t="n">
         <v>0.4</v>
       </c>
-      <c r="D32" s="5" t="n">
+      <c r="D32" s="6" t="n">
         <v>0.449444055557251</v>
       </c>
-      <c r="E32" s="4" t="n">
+      <c r="E32" s="5" t="n">
         <v>13448</v>
       </c>
-      <c r="F32" s="5" t="n">
+      <c r="F32" s="6" t="n">
         <v>11525</v>
       </c>
       <c r="G32" s="4" t="n">
         <v>6</v>
       </c>
-      <c r="H32" s="5" t="n">
+      <c r="H32" s="6" t="n">
         <v>59534</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A33" s="4" t="n">
-        <v>5</v>
-      </c>
-      <c r="B33" s="5" t="n">
-        <v>30</v>
-      </c>
-      <c r="C33" s="4" t="n">
+      <c r="A33" s="5" t="n">
+        <v>5</v>
+      </c>
+      <c r="B33" s="6" t="n">
+        <v>30</v>
+      </c>
+      <c r="C33" s="5" t="n">
         <v>0.5</v>
       </c>
-      <c r="D33" s="5" t="n">
+      <c r="D33" s="6" t="n">
         <v>2.24744009971619</v>
       </c>
-      <c r="E33" s="4" t="n">
+      <c r="E33" s="5" t="n">
         <v>64812</v>
       </c>
-      <c r="F33" s="5" t="n">
+      <c r="F33" s="6" t="n">
         <v>55291</v>
       </c>
       <c r="G33" s="4" t="n">
         <v>7</v>
       </c>
-      <c r="H33" s="5" t="n">
+      <c r="H33" s="6" t="n">
         <v>316379</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A34" s="6" t="s">
+      <c r="A34" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="B34" s="6"/>
-      <c r="C34" s="6"/>
-      <c r="D34" s="7" t="n">
+      <c r="B34" s="7"/>
+      <c r="C34" s="7"/>
+      <c r="D34" s="8" t="n">
         <f aca="false">MIN(D29:D33)</f>
         <v>0.00157856941223145</v>
       </c>
-      <c r="E34" s="7" t="n">
+      <c r="E34" s="8" t="n">
         <f aca="false">MIN(E29:E33)</f>
         <v>44</v>
       </c>
-      <c r="F34" s="7" t="n">
+      <c r="F34" s="8" t="n">
         <f aca="false">MIN(F29:F33)</f>
         <v>13</v>
       </c>
-      <c r="G34" s="7" t="n">
+      <c r="G34" s="8" t="n">
         <f aca="false">MIN(G29:G33)</f>
         <v>3</v>
       </c>
-      <c r="H34" s="7" t="n">
+      <c r="H34" s="8" t="n">
         <f aca="false">MIN(H29:H33)</f>
         <v>71</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A35" s="6" t="s">
+      <c r="A35" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="B35" s="6"/>
-      <c r="C35" s="6"/>
-      <c r="D35" s="7" t="n">
+      <c r="B35" s="7"/>
+      <c r="C35" s="7"/>
+      <c r="D35" s="8" t="n">
         <f aca="false">MAX(D29:D33)</f>
         <v>2.24744009971619</v>
       </c>
-      <c r="E35" s="7" t="n">
+      <c r="E35" s="8" t="n">
         <f aca="false">MAX(E29:E33)</f>
         <v>64812</v>
       </c>
-      <c r="F35" s="7" t="n">
+      <c r="F35" s="8" t="n">
         <f aca="false">MAX(F29:F33)</f>
         <v>55291</v>
       </c>
-      <c r="G35" s="7" t="n">
+      <c r="G35" s="8" t="n">
         <f aca="false">MAX(G29:G33)</f>
         <v>7</v>
       </c>
-      <c r="H35" s="7" t="n">
+      <c r="H35" s="8" t="n">
         <f aca="false">MAX(H29:H33)</f>
         <v>316379</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A36" s="6" t="s">
+      <c r="A36" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="B36" s="6"/>
-      <c r="C36" s="6"/>
-      <c r="D36" s="7" t="n">
+      <c r="B36" s="7"/>
+      <c r="C36" s="7"/>
+      <c r="D36" s="8" t="n">
         <f aca="false">AVERAGE(D29:D33)</f>
         <v>0.552222442626953</v>
       </c>
-      <c r="E36" s="7" t="n">
+      <c r="E36" s="8" t="n">
         <f aca="false">AVERAGE(E29:E33)</f>
         <v>16046.2</v>
       </c>
-      <c r="F36" s="7" t="n">
+      <c r="F36" s="8" t="n">
         <f aca="false">AVERAGE(F29:F33)</f>
         <v>13678.8</v>
       </c>
-      <c r="G36" s="7" t="n">
+      <c r="G36" s="8" t="n">
         <f aca="false">AVERAGE(G29:G33)</f>
         <v>5</v>
       </c>
-      <c r="H36" s="7" t="n">
+      <c r="H36" s="8" t="n">
         <f aca="false">AVERAGE(H29:H33)</f>
         <v>76906.8</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A37" s="6" t="s">
+      <c r="A37" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="B37" s="6"/>
-      <c r="C37" s="6"/>
-      <c r="D37" s="7" t="n">
+      <c r="B37" s="7"/>
+      <c r="C37" s="7"/>
+      <c r="D37" s="8" t="n">
         <f aca="false">MEDIAN(D29:D33)</f>
         <v>0.0594370365142822</v>
       </c>
-      <c r="E37" s="7" t="n">
+      <c r="E37" s="8" t="n">
         <f aca="false">MEDIAN(E29:E33)</f>
         <v>1849</v>
       </c>
-      <c r="F37" s="7" t="n">
+      <c r="F37" s="8" t="n">
         <f aca="false">MEDIAN(F29:F33)</f>
         <v>1523</v>
       </c>
-      <c r="G37" s="7" t="n">
+      <c r="G37" s="8" t="n">
         <f aca="false">MEDIAN(G29:G33)</f>
         <v>5</v>
       </c>
-      <c r="H37" s="7" t="n">
+      <c r="H37" s="8" t="n">
         <f aca="false">MEDIAN(H29:H33)</f>
         <v>8251</v>
       </c>
@@ -1254,7 +1260,7 @@
       <c r="F40" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="G40" s="3" t="s">
+      <c r="G40" s="4" t="s">
         <v>8</v>
       </c>
       <c r="H40" s="3" t="s">
@@ -1262,239 +1268,239 @@
       </c>
     </row>
     <row r="41" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A41" s="4" t="n">
+      <c r="A41" s="5" t="n">
         <v>1</v>
       </c>
-      <c r="B41" s="5" t="n">
-        <v>30</v>
-      </c>
-      <c r="C41" s="4" t="n">
+      <c r="B41" s="6" t="n">
+        <v>30</v>
+      </c>
+      <c r="C41" s="5" t="n">
         <v>0.1</v>
       </c>
-      <c r="D41" s="5" t="n">
+      <c r="D41" s="6" t="n">
         <v>0.00127696990966797</v>
       </c>
-      <c r="E41" s="4" t="n">
+      <c r="E41" s="5" t="n">
         <v>35</v>
       </c>
-      <c r="F41" s="5" t="n">
+      <c r="F41" s="6" t="n">
         <v>4</v>
       </c>
       <c r="G41" s="4" t="n">
         <v>3</v>
       </c>
-      <c r="H41" s="5" t="n">
+      <c r="H41" s="6" t="n">
         <v>52</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A42" s="4" t="n">
+      <c r="A42" s="5" t="n">
         <v>2</v>
       </c>
-      <c r="B42" s="5" t="n">
-        <v>30</v>
-      </c>
-      <c r="C42" s="4" t="n">
+      <c r="B42" s="6" t="n">
+        <v>30</v>
+      </c>
+      <c r="C42" s="5" t="n">
         <v>0.2</v>
       </c>
-      <c r="D42" s="5" t="n">
+      <c r="D42" s="6" t="n">
         <v>0.00825858116149902</v>
       </c>
-      <c r="E42" s="4" t="n">
+      <c r="E42" s="5" t="n">
         <v>276</v>
       </c>
-      <c r="F42" s="5" t="n">
+      <c r="F42" s="6" t="n">
         <v>222</v>
       </c>
       <c r="G42" s="4" t="n">
         <v>4</v>
       </c>
-      <c r="H42" s="5" t="n">
+      <c r="H42" s="6" t="n">
         <v>657</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A43" s="4" t="n">
-        <v>3</v>
-      </c>
-      <c r="B43" s="5" t="n">
-        <v>30</v>
-      </c>
-      <c r="C43" s="4" t="n">
+      <c r="A43" s="5" t="n">
+        <v>3</v>
+      </c>
+      <c r="B43" s="6" t="n">
+        <v>30</v>
+      </c>
+      <c r="C43" s="5" t="n">
         <v>0.3</v>
       </c>
-      <c r="D43" s="5" t="n">
+      <c r="D43" s="6" t="n">
         <v>0.0500688552856445</v>
       </c>
-      <c r="E43" s="4" t="n">
+      <c r="E43" s="5" t="n">
         <v>1532</v>
       </c>
-      <c r="F43" s="5" t="n">
+      <c r="F43" s="6" t="n">
         <v>1310</v>
       </c>
       <c r="G43" s="4" t="n">
         <v>5</v>
       </c>
-      <c r="H43" s="5" t="n">
+      <c r="H43" s="6" t="n">
         <v>6300</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A44" s="4" t="n">
+      <c r="A44" s="5" t="n">
         <v>4</v>
       </c>
-      <c r="B44" s="5" t="n">
-        <v>30</v>
-      </c>
-      <c r="C44" s="4" t="n">
+      <c r="B44" s="6" t="n">
+        <v>30</v>
+      </c>
+      <c r="C44" s="5" t="n">
         <v>0.4</v>
       </c>
-      <c r="D44" s="5" t="n">
+      <c r="D44" s="6" t="n">
         <v>0.161075830459595</v>
       </c>
-      <c r="E44" s="4" t="n">
+      <c r="E44" s="5" t="n">
         <v>4423</v>
       </c>
-      <c r="F44" s="5" t="n">
+      <c r="F44" s="6" t="n">
         <v>3678</v>
       </c>
       <c r="G44" s="4" t="n">
         <v>6</v>
       </c>
-      <c r="H44" s="5" t="n">
+      <c r="H44" s="6" t="n">
         <v>26522</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A45" s="4" t="n">
-        <v>5</v>
-      </c>
-      <c r="B45" s="5" t="n">
-        <v>30</v>
-      </c>
-      <c r="C45" s="4" t="n">
+      <c r="A45" s="5" t="n">
+        <v>5</v>
+      </c>
+      <c r="B45" s="6" t="n">
+        <v>30</v>
+      </c>
+      <c r="C45" s="5" t="n">
         <v>0.5</v>
       </c>
-      <c r="D45" s="5" t="n">
+      <c r="D45" s="6" t="n">
         <v>1.93194222450256</v>
       </c>
-      <c r="E45" s="4" t="n">
+      <c r="E45" s="5" t="n">
         <v>55011</v>
       </c>
-      <c r="F45" s="5" t="n">
+      <c r="F45" s="6" t="n">
         <v>46649</v>
       </c>
       <c r="G45" s="4" t="n">
         <v>7</v>
       </c>
-      <c r="H45" s="5" t="n">
+      <c r="H45" s="6" t="n">
         <v>278196</v>
       </c>
     </row>
     <row r="46" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A46" s="6" t="s">
+      <c r="A46" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="B46" s="6"/>
-      <c r="C46" s="6"/>
-      <c r="D46" s="7" t="n">
+      <c r="B46" s="7"/>
+      <c r="C46" s="7"/>
+      <c r="D46" s="8" t="n">
         <f aca="false">MIN(D41:D45)</f>
         <v>0.00127696990966797</v>
       </c>
-      <c r="E46" s="7" t="n">
+      <c r="E46" s="8" t="n">
         <f aca="false">MIN(E41:E45)</f>
         <v>35</v>
       </c>
-      <c r="F46" s="7" t="n">
+      <c r="F46" s="8" t="n">
         <f aca="false">MIN(F41:F45)</f>
         <v>4</v>
       </c>
-      <c r="G46" s="7" t="n">
+      <c r="G46" s="8" t="n">
         <f aca="false">MIN(G41:G45)</f>
         <v>3</v>
       </c>
-      <c r="H46" s="7" t="n">
+      <c r="H46" s="8" t="n">
         <f aca="false">MIN(H41:H45)</f>
         <v>52</v>
       </c>
     </row>
     <row r="47" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A47" s="6" t="s">
+      <c r="A47" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="B47" s="6"/>
-      <c r="C47" s="6"/>
-      <c r="D47" s="7" t="n">
+      <c r="B47" s="7"/>
+      <c r="C47" s="7"/>
+      <c r="D47" s="8" t="n">
         <f aca="false">MAX(D41:D45)</f>
         <v>1.93194222450256</v>
       </c>
-      <c r="E47" s="7" t="n">
+      <c r="E47" s="8" t="n">
         <f aca="false">MAX(E41:E45)</f>
         <v>55011</v>
       </c>
-      <c r="F47" s="7" t="n">
+      <c r="F47" s="8" t="n">
         <f aca="false">MAX(F41:F45)</f>
         <v>46649</v>
       </c>
-      <c r="G47" s="7" t="n">
+      <c r="G47" s="8" t="n">
         <f aca="false">MAX(G41:G45)</f>
         <v>7</v>
       </c>
-      <c r="H47" s="7" t="n">
+      <c r="H47" s="8" t="n">
         <f aca="false">MAX(H41:H45)</f>
         <v>278196</v>
       </c>
     </row>
     <row r="48" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A48" s="6" t="s">
+      <c r="A48" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="B48" s="6"/>
-      <c r="C48" s="6"/>
-      <c r="D48" s="7" t="n">
+      <c r="B48" s="7"/>
+      <c r="C48" s="7"/>
+      <c r="D48" s="8" t="n">
         <f aca="false">AVERAGE(D41:D45)</f>
         <v>0.430524492263794</v>
       </c>
-      <c r="E48" s="7" t="n">
+      <c r="E48" s="8" t="n">
         <f aca="false">AVERAGE(E41:E45)</f>
         <v>12255.4</v>
       </c>
-      <c r="F48" s="7" t="n">
+      <c r="F48" s="8" t="n">
         <f aca="false">AVERAGE(F41:F45)</f>
         <v>10372.6</v>
       </c>
-      <c r="G48" s="7" t="n">
+      <c r="G48" s="8" t="n">
         <f aca="false">AVERAGE(G41:G45)</f>
         <v>5</v>
       </c>
-      <c r="H48" s="7" t="n">
+      <c r="H48" s="8" t="n">
         <f aca="false">AVERAGE(H41:H45)</f>
         <v>62345.4</v>
       </c>
     </row>
     <row r="49" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A49" s="6" t="s">
+      <c r="A49" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="B49" s="6"/>
-      <c r="C49" s="6"/>
-      <c r="D49" s="7" t="n">
+      <c r="B49" s="7"/>
+      <c r="C49" s="7"/>
+      <c r="D49" s="8" t="n">
         <f aca="false">MEDIAN(D41:D45)</f>
         <v>0.0500688552856445</v>
       </c>
-      <c r="E49" s="7" t="n">
+      <c r="E49" s="8" t="n">
         <f aca="false">MEDIAN(E41:E45)</f>
         <v>1532</v>
       </c>
-      <c r="F49" s="7" t="n">
+      <c r="F49" s="8" t="n">
         <f aca="false">MEDIAN(F41:F45)</f>
         <v>1310</v>
       </c>
-      <c r="G49" s="7" t="n">
+      <c r="G49" s="8" t="n">
         <f aca="false">MEDIAN(G41:G45)</f>
         <v>5</v>
       </c>
-      <c r="H49" s="7" t="n">
+      <c r="H49" s="8" t="n">
         <f aca="false">MEDIAN(H41:H45)</f>
         <v>6300</v>
       </c>
@@ -1533,7 +1539,7 @@
       <c r="F52" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="G52" s="3" t="s">
+      <c r="G52" s="4" t="s">
         <v>8</v>
       </c>
       <c r="H52" s="3" t="s">
@@ -1541,239 +1547,239 @@
       </c>
     </row>
     <row r="53" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A53" s="4" t="n">
+      <c r="A53" s="5" t="n">
         <v>1</v>
       </c>
-      <c r="B53" s="5" t="n">
-        <v>30</v>
-      </c>
-      <c r="C53" s="4" t="n">
+      <c r="B53" s="6" t="n">
+        <v>30</v>
+      </c>
+      <c r="C53" s="5" t="n">
         <v>0.1</v>
       </c>
-      <c r="D53" s="5" t="n">
+      <c r="D53" s="6" t="n">
         <v>0.00151324272155762</v>
       </c>
-      <c r="E53" s="4" t="n">
+      <c r="E53" s="5" t="n">
         <v>42</v>
       </c>
-      <c r="F53" s="5" t="n">
+      <c r="F53" s="6" t="n">
         <v>11</v>
       </c>
       <c r="G53" s="4" t="n">
         <v>3</v>
       </c>
-      <c r="H53" s="5" t="n">
+      <c r="H53" s="6" t="n">
         <v>69</v>
       </c>
     </row>
     <row r="54" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A54" s="4" t="n">
+      <c r="A54" s="5" t="n">
         <v>2</v>
       </c>
-      <c r="B54" s="5" t="n">
-        <v>30</v>
-      </c>
-      <c r="C54" s="4" t="n">
+      <c r="B54" s="6" t="n">
+        <v>30</v>
+      </c>
+      <c r="C54" s="5" t="n">
         <v>0.2</v>
       </c>
-      <c r="D54" s="5" t="n">
+      <c r="D54" s="6" t="n">
         <v>0.00538158416748047</v>
       </c>
-      <c r="E54" s="4" t="n">
+      <c r="E54" s="5" t="n">
         <v>156</v>
       </c>
-      <c r="F54" s="5" t="n">
+      <c r="F54" s="6" t="n">
         <v>106</v>
       </c>
       <c r="G54" s="4" t="n">
         <v>4</v>
       </c>
-      <c r="H54" s="5" t="n">
+      <c r="H54" s="6" t="n">
         <v>521</v>
       </c>
     </row>
     <row r="55" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A55" s="4" t="n">
-        <v>3</v>
-      </c>
-      <c r="B55" s="5" t="n">
-        <v>30</v>
-      </c>
-      <c r="C55" s="4" t="n">
+      <c r="A55" s="5" t="n">
+        <v>3</v>
+      </c>
+      <c r="B55" s="6" t="n">
+        <v>30</v>
+      </c>
+      <c r="C55" s="5" t="n">
         <v>0.3</v>
       </c>
-      <c r="D55" s="5" t="n">
+      <c r="D55" s="6" t="n">
         <v>0.0396368503570557</v>
       </c>
-      <c r="E55" s="4" t="n">
+      <c r="E55" s="5" t="n">
         <v>1222</v>
       </c>
-      <c r="F55" s="5" t="n">
+      <c r="F55" s="6" t="n">
         <v>1028</v>
       </c>
       <c r="G55" s="4" t="n">
         <v>5</v>
       </c>
-      <c r="H55" s="5" t="n">
+      <c r="H55" s="6" t="n">
         <v>4536</v>
       </c>
     </row>
     <row r="56" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A56" s="4" t="n">
+      <c r="A56" s="5" t="n">
         <v>4</v>
       </c>
-      <c r="B56" s="5" t="n">
-        <v>30</v>
-      </c>
-      <c r="C56" s="4" t="n">
+      <c r="B56" s="6" t="n">
+        <v>30</v>
+      </c>
+      <c r="C56" s="5" t="n">
         <v>0.4</v>
       </c>
-      <c r="D56" s="5" t="n">
+      <c r="D56" s="6" t="n">
         <v>0.0593504905700684</v>
       </c>
-      <c r="E56" s="4" t="n">
+      <c r="E56" s="5" t="n">
         <v>1538</v>
       </c>
-      <c r="F56" s="5" t="n">
+      <c r="F56" s="6" t="n">
         <v>1273</v>
       </c>
       <c r="G56" s="4" t="n">
         <v>6</v>
       </c>
-      <c r="H56" s="5" t="n">
+      <c r="H56" s="6" t="n">
         <v>9741</v>
       </c>
     </row>
     <row r="57" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A57" s="4" t="n">
-        <v>5</v>
-      </c>
-      <c r="B57" s="5" t="n">
-        <v>30</v>
-      </c>
-      <c r="C57" s="4" t="n">
+      <c r="A57" s="5" t="n">
+        <v>5</v>
+      </c>
+      <c r="B57" s="6" t="n">
+        <v>30</v>
+      </c>
+      <c r="C57" s="5" t="n">
         <v>0.5</v>
       </c>
-      <c r="D57" s="5" t="n">
+      <c r="D57" s="6" t="n">
         <v>1.12483596801758</v>
       </c>
-      <c r="E57" s="4" t="n">
+      <c r="E57" s="5" t="n">
         <v>31698</v>
       </c>
-      <c r="F57" s="5" t="n">
+      <c r="F57" s="6" t="n">
         <v>25525</v>
       </c>
       <c r="G57" s="4" t="n">
         <v>7</v>
       </c>
-      <c r="H57" s="5" t="n">
+      <c r="H57" s="6" t="n">
         <v>185388</v>
       </c>
     </row>
     <row r="58" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A58" s="6" t="s">
+      <c r="A58" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="B58" s="6"/>
-      <c r="C58" s="6"/>
-      <c r="D58" s="7" t="n">
+      <c r="B58" s="7"/>
+      <c r="C58" s="7"/>
+      <c r="D58" s="8" t="n">
         <f aca="false">MIN(D53:D57)</f>
         <v>0.00151324272155762</v>
       </c>
-      <c r="E58" s="7" t="n">
+      <c r="E58" s="8" t="n">
         <f aca="false">MIN(E53:E57)</f>
         <v>42</v>
       </c>
-      <c r="F58" s="7" t="n">
+      <c r="F58" s="8" t="n">
         <f aca="false">MIN(F52:F57)</f>
         <v>11</v>
       </c>
-      <c r="G58" s="7" t="n">
+      <c r="G58" s="8" t="n">
         <f aca="false">MIN(G53:G57)</f>
         <v>3</v>
       </c>
-      <c r="H58" s="7" t="n">
+      <c r="H58" s="8" t="n">
         <f aca="false">MIN(H53:H57)</f>
         <v>69</v>
       </c>
     </row>
     <row r="59" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A59" s="6" t="s">
+      <c r="A59" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="B59" s="6"/>
-      <c r="C59" s="6"/>
-      <c r="D59" s="7" t="n">
+      <c r="B59" s="7"/>
+      <c r="C59" s="7"/>
+      <c r="D59" s="8" t="n">
         <f aca="false">MAX(D53:D57)</f>
         <v>1.12483596801758</v>
       </c>
-      <c r="E59" s="7" t="n">
+      <c r="E59" s="8" t="n">
         <f aca="false">MAX(E53:E57)</f>
         <v>31698</v>
       </c>
-      <c r="F59" s="7" t="n">
+      <c r="F59" s="8" t="n">
         <f aca="false">MAX(F52:F57)</f>
         <v>25525</v>
       </c>
-      <c r="G59" s="7" t="n">
+      <c r="G59" s="8" t="n">
         <f aca="false">MAX(G53:G57)</f>
         <v>7</v>
       </c>
-      <c r="H59" s="7" t="n">
+      <c r="H59" s="8" t="n">
         <f aca="false">MAX(H53:H57)</f>
         <v>185388</v>
       </c>
     </row>
     <row r="60" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A60" s="6" t="s">
+      <c r="A60" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="B60" s="6"/>
-      <c r="C60" s="6"/>
-      <c r="D60" s="7" t="n">
+      <c r="B60" s="7"/>
+      <c r="C60" s="7"/>
+      <c r="D60" s="8" t="n">
         <f aca="false">AVERAGE(D53:D57)</f>
         <v>0.246143627166748</v>
       </c>
-      <c r="E60" s="7" t="n">
+      <c r="E60" s="8" t="n">
         <f aca="false">AVERAGE(E53:E57)</f>
         <v>6931.2</v>
       </c>
-      <c r="F60" s="7" t="n">
+      <c r="F60" s="8" t="n">
         <f aca="false">AVERAGE(F52:F57)</f>
         <v>5588.6</v>
       </c>
-      <c r="G60" s="7" t="n">
+      <c r="G60" s="8" t="n">
         <f aca="false">AVERAGE(G53:G57)</f>
         <v>5</v>
       </c>
-      <c r="H60" s="7" t="n">
+      <c r="H60" s="8" t="n">
         <f aca="false">AVERAGE(H53:H57)</f>
         <v>40051</v>
       </c>
     </row>
     <row r="61" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A61" s="6" t="s">
+      <c r="A61" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="B61" s="6"/>
-      <c r="C61" s="6"/>
-      <c r="D61" s="7" t="n">
+      <c r="B61" s="7"/>
+      <c r="C61" s="7"/>
+      <c r="D61" s="8" t="n">
         <f aca="false">MEDIAN(D53:D57)</f>
         <v>0.0396368503570557</v>
       </c>
-      <c r="E61" s="7" t="n">
+      <c r="E61" s="8" t="n">
         <f aca="false">MEDIAN(E53:E57)</f>
         <v>1222</v>
       </c>
-      <c r="F61" s="7" t="n">
+      <c r="F61" s="8" t="n">
         <f aca="false">MEDIAN(F52:F57)</f>
         <v>1028</v>
       </c>
-      <c r="G61" s="7" t="n">
+      <c r="G61" s="8" t="n">
         <f aca="false">MEDIAN(G53:G57)</f>
         <v>5</v>
       </c>
-      <c r="H61" s="7" t="n">
+      <c r="H61" s="8" t="n">
         <f aca="false">MEDIAN(H53:H57)</f>
         <v>4536</v>
       </c>

</xml_diff>